<commit_message>
implemented a task with an asterisk related to promotional dishes
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sonic_tim\PycharmProjects\YLabProject\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708ED897-F820-4447-BCC0-1AFDD8F76C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADB47C5-DCC9-47F9-A99F-83E5540E3921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
FIXED A PROBLEM WITH UPDATING A FILE OUTSIDE THE CONTAINER. THE UPDATE IS WORKING STABLY
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sonic_tim\PycharmProjects\YLabProject\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ADB47C5-DCC9-47F9-A99F-83E5540E3921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2031510-6BC3-4AB7-9206-C787A13AC562}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
@@ -687,7 +687,9 @@
       <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2">
+        <v>10</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">

</xml_diff>

<commit_message>
IMPLEMENTED `Updating the menu from google sheets every 15 seconds`. Look README.md
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sonic_tim\PycharmProjects\YLabProject\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2031510-6BC3-4AB7-9206-C787A13AC562}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FCF6AA-71F5-4725-92DD-623CB88C6254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
@@ -687,9 +687,7 @@
       <c r="F9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="2">
-        <v>10</v>
-      </c>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">

</xml_diff>

<commit_message>
slightly updated `README.md `; changed the sequence of launching services in `docker-compose.yaml`
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sonic_tim\PycharmProjects\YLabProject\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FCF6AA-71F5-4725-92DD-623CB88C6254}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED452D-7719-45BD-91B1-4E08A2D81ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Fixed `when trying to add a new menu (id: 05360824-639e-471c-a44f-127064d32a98 title: new menu description: hbo menu) ) via xlxs file I get 500 error Internal Server Error if you remove the id, the error goes away, but the new menu is not added`
</commit_message>
<xml_diff>
--- a/admin/Menu.xlsx
+++ b/admin/Menu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\sonic_tim\PycharmProjects\YLabProject\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52ED452D-7719-45BD-91B1-4E08A2D81ACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1364B8D7-536E-41DF-9C70-BA354064EF6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
   <si>
     <t>Холодные закуски</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>Меню</t>
+  </si>
+  <si>
+    <t>05360824-639e-471c-a44f-127064d32a98</t>
+  </si>
+  <si>
+    <t>новое меню</t>
+  </si>
+  <si>
+    <t>меню нво</t>
   </si>
 </sst>
 </file>
@@ -529,7 +538,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="15" customHeight="1"/>
@@ -836,7 +845,17 @@
       </c>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1"/>
+    <row r="19" spans="1:7" ht="15.75" customHeight="1">
+      <c r="A19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="21" spans="1:7" ht="15.75" customHeight="1"/>
     <row r="22" spans="1:7" ht="15.75" customHeight="1"/>
@@ -1821,5 +1840,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>